<commit_message>
Update Function Progress Checker.xlsx
</commit_message>
<xml_diff>
--- a/Function Progress Checker.xlsx
+++ b/Function Progress Checker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwlroda/Documents/GitHub/mjnwlc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\C++\MipsSim\mjnwlc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A8D94C-EDAB-7048-A29D-76B1F8A0A927}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C384A95-AEC1-49CB-8131-748F6E41F61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{DE50BC15-ADE5-4BB9-9D10-6F39E6D74606}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE50BC15-ADE5-4BB9-9D10-6F39E6D74606}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="131">
   <si>
     <t>Code</t>
   </si>
@@ -417,14 +417,20 @@
     <t>Fn Creation</t>
   </si>
   <si>
-    <t>Tested</t>
+    <t>Primary Tested</t>
+  </si>
+  <si>
+    <t>Edge Tested</t>
+  </si>
+  <si>
+    <t>d (jr = 0 only)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -857,27 +863,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4F9F8A-A699-4B69-A229-2709480D0D98}">
-  <dimension ref="A1:F59"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="86" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="19" thickBot="1">
+    <row r="2" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -896,8 +906,11 @@
       <c r="F2" s="8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="19" thickBot="1">
+      <c r="G2" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -913,11 +926,9 @@
       <c r="E3" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="19" thickBot="1">
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -934,7 +945,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="19" thickBot="1">
+    <row r="5" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -951,7 +962,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="19" thickBot="1">
+    <row r="6" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -967,11 +978,9 @@
       <c r="E6" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="19" thickBot="1">
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -988,7 +997,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19" thickBot="1">
+    <row r="8" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1005,7 +1014,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19" thickBot="1">
+    <row r="9" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -1022,7 +1031,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="19" thickBot="1">
+    <row r="10" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
@@ -1039,7 +1048,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="19" thickBot="1">
+    <row r="11" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -1056,7 +1065,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19" thickBot="1">
+    <row r="12" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -1073,7 +1082,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="19" thickBot="1">
+    <row r="13" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -1090,7 +1099,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="19" thickBot="1">
+    <row r="14" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
@@ -1107,7 +1116,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="19" thickBot="1">
+    <row r="15" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1124,7 +1133,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="19" thickBot="1">
+    <row r="16" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
@@ -1141,7 +1150,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="19" thickBot="1">
+    <row r="17" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -1155,7 +1164,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="19" thickBot="1">
+    <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -1169,7 +1178,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="19" thickBot="1">
+    <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
@@ -1186,7 +1195,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="19" thickBot="1">
+    <row r="20" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>41</v>
       </c>
@@ -1203,7 +1212,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="19" thickBot="1">
+    <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
@@ -1220,7 +1229,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="19" thickBot="1">
+    <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>45</v>
       </c>
@@ -1237,10 +1246,10 @@
         <v>122</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="19" thickBot="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>47</v>
       </c>
@@ -1257,7 +1266,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="19" thickBot="1">
+    <row r="24" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
@@ -1271,7 +1280,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="19" thickBot="1">
+    <row r="25" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>51</v>
       </c>
@@ -1285,7 +1294,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="19" thickBot="1">
+    <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>53</v>
       </c>
@@ -1299,7 +1308,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="19" thickBot="1">
+    <row r="27" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>55</v>
       </c>
@@ -1315,8 +1324,11 @@
       <c r="E27" s="9" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="19" thickBot="1">
+      <c r="F27" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>57</v>
       </c>
@@ -1333,7 +1345,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="19" thickBot="1">
+    <row r="29" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>59</v>
       </c>
@@ -1347,7 +1359,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="19" thickBot="1">
+    <row r="30" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>62</v>
       </c>
@@ -1361,7 +1373,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="19" thickBot="1">
+    <row r="31" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>64</v>
       </c>
@@ -1378,7 +1390,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="19" thickBot="1">
+    <row r="32" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>66</v>
       </c>
@@ -1395,7 +1407,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="19" thickBot="1">
+    <row r="33" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>68</v>
       </c>
@@ -1412,7 +1424,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="19" thickBot="1">
+    <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>70</v>
       </c>
@@ -1429,7 +1441,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="19" thickBot="1">
+    <row r="35" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>72</v>
       </c>
@@ -1443,7 +1455,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="19" thickBot="1">
+    <row r="36" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>74</v>
       </c>
@@ -1457,7 +1469,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="19" thickBot="1">
+    <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>76</v>
       </c>
@@ -1473,8 +1485,11 @@
       <c r="E37" s="9" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="19" thickBot="1">
+      <c r="F37" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>78</v>
       </c>
@@ -1491,7 +1506,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="19" thickBot="1">
+    <row r="39" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>80</v>
       </c>
@@ -1508,7 +1523,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="19" thickBot="1">
+    <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>82</v>
       </c>
@@ -1522,7 +1537,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="19" thickBot="1">
+    <row r="41" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>84</v>
       </c>
@@ -1539,7 +1554,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="19" thickBot="1">
+    <row r="42" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>86</v>
       </c>
@@ -1556,7 +1571,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="19" thickBot="1">
+    <row r="43" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>88</v>
       </c>
@@ -1573,7 +1588,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="19" thickBot="1">
+    <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>90</v>
       </c>
@@ -1590,7 +1605,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="19" thickBot="1">
+    <row r="45" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>92</v>
       </c>
@@ -1607,7 +1622,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="19" thickBot="1">
+    <row r="46" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>94</v>
       </c>
@@ -1624,7 +1639,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="19" thickBot="1">
+    <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>96</v>
       </c>
@@ -1641,7 +1656,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="19" thickBot="1">
+    <row r="48" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>98</v>
       </c>
@@ -1658,7 +1673,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="19" thickBot="1">
+    <row r="49" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>99</v>
       </c>
@@ -1675,7 +1690,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="19" thickBot="1">
+    <row r="50" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>101</v>
       </c>
@@ -1692,7 +1707,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="19" thickBot="1">
+    <row r="51" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>103</v>
       </c>
@@ -1709,7 +1724,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="19" thickBot="1">
+    <row r="52" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>105</v>
       </c>
@@ -1726,7 +1741,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="19" thickBot="1">
+    <row r="53" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>107</v>
       </c>
@@ -1743,7 +1758,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="19" thickBot="1">
+    <row r="54" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>109</v>
       </c>
@@ -1760,7 +1775,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="19" thickBot="1">
+    <row r="55" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>111</v>
       </c>
@@ -1777,7 +1792,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="19" thickBot="1">
+    <row r="56" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>113</v>
       </c>
@@ -1788,7 +1803,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="19" thickBot="1">
+    <row r="57" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>116</v>
       </c>
@@ -1797,7 +1812,7 @@
       </c>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:5" ht="19" thickBot="1">
+    <row r="58" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>118</v>
       </c>
@@ -1806,7 +1821,7 @@
       </c>
       <c r="C58" s="5"/>
     </row>
-    <row r="59" spans="1:5" ht="19" thickBot="1">
+    <row r="59" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
testing of addiu addi sub subu
</commit_message>
<xml_diff>
--- a/Function Progress Checker.xlsx
+++ b/Function Progress Checker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cwlroda/Documents/GitHub/mjnwlc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\C++\MipsSim\mjnwlc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C3AD99-FD1C-BA44-AEE8-FAA7EF0A51EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158C40E4-14CD-472A-A4B2-DE091D94B3CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17480" windowHeight="20540" activeTab="1" xr2:uid="{DE50BC15-ADE5-4BB9-9D10-6F39E6D74606}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DE50BC15-ADE5-4BB9-9D10-6F39E6D74606}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="168">
   <si>
     <t>Code</t>
   </si>
@@ -445,12 +445,6 @@
     <t>Exit program</t>
   </si>
   <si>
-    <t>0x10000000</t>
-  </si>
-  <si>
-    <t>Jump to first instruction</t>
-  </si>
-  <si>
     <t>Address is stored in R31</t>
   </si>
   <si>
@@ -469,15 +463,9 @@
     <t>Error: Arithmetic overflow</t>
   </si>
   <si>
-    <t>0x7000000 + 0xFFFFFFF</t>
-  </si>
-  <si>
     <t>0x8000000 + 0x1</t>
   </si>
   <si>
-    <t>0x1 + 0x80000000</t>
-  </si>
-  <si>
     <t>0xFFFFFFFF + 0x80000001</t>
   </si>
   <si>
@@ -521,13 +509,40 @@
   </si>
   <si>
     <t>Jump to out of memory</t>
+  </si>
+  <si>
+    <t>Return Code</t>
+  </si>
+  <si>
+    <t>Jump to 2 instructions later</t>
+  </si>
+  <si>
+    <t>success BUT no delay slot!!</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>Normal Case</t>
+  </si>
+  <si>
+    <t>0x70000000 + 0x0FFFFFFF</t>
+  </si>
+  <si>
+    <t>normal case</t>
+  </si>
+  <si>
+    <t>0x7000000 + 0x0FFFFFFF</t>
+  </si>
+  <si>
+    <t>0XFFFFFFFF + 0xFFFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -987,25 +1002,25 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="2"/>
+    <col min="5" max="5" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" thickBot="1">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="19" thickBot="1">
+    <row r="2" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1046,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19" thickBot="1">
+    <row r="3" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1051,7 +1066,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19" thickBot="1">
+    <row r="4" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1074,7 +1089,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19" thickBot="1">
+    <row r="5" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1097,7 +1112,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19" thickBot="1">
+    <row r="6" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1117,7 +1132,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19" thickBot="1">
+    <row r="7" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1137,7 +1152,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19" thickBot="1">
+    <row r="8" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1157,7 +1172,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="19" thickBot="1">
+    <row r="9" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -1174,7 +1189,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19" thickBot="1">
+    <row r="10" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
@@ -1191,7 +1206,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19" thickBot="1">
+    <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -1208,7 +1223,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="19" thickBot="1">
+    <row r="12" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -1225,7 +1240,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="19" thickBot="1">
+    <row r="13" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -1242,7 +1257,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="19" thickBot="1">
+    <row r="14" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
@@ -1259,7 +1274,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="19" thickBot="1">
+    <row r="15" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1276,7 +1291,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="19" thickBot="1">
+    <row r="16" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
@@ -1293,7 +1308,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="19" thickBot="1">
+    <row r="17" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -1310,7 +1325,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="19" thickBot="1">
+    <row r="18" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -1327,7 +1342,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="19" thickBot="1">
+    <row r="19" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
@@ -1344,7 +1359,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="19" thickBot="1">
+    <row r="20" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>41</v>
       </c>
@@ -1361,7 +1376,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="19" thickBot="1">
+    <row r="21" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
@@ -1378,7 +1393,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="19" thickBot="1">
+    <row r="22" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>45</v>
       </c>
@@ -1398,7 +1413,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="19" thickBot="1">
+    <row r="23" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>47</v>
       </c>
@@ -1415,7 +1430,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="19" thickBot="1">
+    <row r="24" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
@@ -1432,7 +1447,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="19" thickBot="1">
+    <row r="25" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>51</v>
       </c>
@@ -1449,7 +1464,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="19" thickBot="1">
+    <row r="26" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>53</v>
       </c>
@@ -1466,7 +1481,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="19" thickBot="1">
+    <row r="27" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>55</v>
       </c>
@@ -1489,7 +1504,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="19" thickBot="1">
+    <row r="28" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>57</v>
       </c>
@@ -1506,7 +1521,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="19" thickBot="1">
+    <row r="29" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>59</v>
       </c>
@@ -1520,7 +1535,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="19" thickBot="1">
+    <row r="30" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>62</v>
       </c>
@@ -1534,7 +1549,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="19" thickBot="1">
+    <row r="31" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>64</v>
       </c>
@@ -1551,7 +1566,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="19" thickBot="1">
+    <row r="32" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>66</v>
       </c>
@@ -1568,7 +1583,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="19" thickBot="1">
+    <row r="33" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>68</v>
       </c>
@@ -1585,7 +1600,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="19" thickBot="1">
+    <row r="34" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>70</v>
       </c>
@@ -1602,7 +1617,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="19" thickBot="1">
+    <row r="35" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>72</v>
       </c>
@@ -1619,7 +1634,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="19" thickBot="1">
+    <row r="36" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>74</v>
       </c>
@@ -1636,7 +1651,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="19" thickBot="1">
+    <row r="37" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>76</v>
       </c>
@@ -1659,7 +1674,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="19" thickBot="1">
+    <row r="38" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>78</v>
       </c>
@@ -1679,7 +1694,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="19" thickBot="1">
+    <row r="39" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>80</v>
       </c>
@@ -1696,7 +1711,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="19" thickBot="1">
+    <row r="40" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>82</v>
       </c>
@@ -1713,7 +1728,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="19" thickBot="1">
+    <row r="41" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>84</v>
       </c>
@@ -1730,7 +1745,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="19" thickBot="1">
+    <row r="42" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>86</v>
       </c>
@@ -1747,7 +1762,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="19" thickBot="1">
+    <row r="43" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>88</v>
       </c>
@@ -1764,7 +1779,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="19" thickBot="1">
+    <row r="44" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>90</v>
       </c>
@@ -1781,7 +1796,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="19" thickBot="1">
+    <row r="45" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>92</v>
       </c>
@@ -1798,7 +1813,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="19" thickBot="1">
+    <row r="46" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>94</v>
       </c>
@@ -1815,7 +1830,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="19" thickBot="1">
+    <row r="47" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>96</v>
       </c>
@@ -1832,7 +1847,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="19" thickBot="1">
+    <row r="48" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>98</v>
       </c>
@@ -1849,7 +1864,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="19" thickBot="1">
+    <row r="49" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>99</v>
       </c>
@@ -1866,7 +1881,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="19" thickBot="1">
+    <row r="50" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>101</v>
       </c>
@@ -1883,7 +1898,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="19" thickBot="1">
+    <row r="51" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>103</v>
       </c>
@@ -1903,7 +1918,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="19" thickBot="1">
+    <row r="52" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>105</v>
       </c>
@@ -1923,7 +1938,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="19" thickBot="1">
+    <row r="53" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>107</v>
       </c>
@@ -1940,7 +1955,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="19" thickBot="1">
+    <row r="54" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>109</v>
       </c>
@@ -1960,7 +1975,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="19" thickBot="1">
+    <row r="55" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>111</v>
       </c>
@@ -1980,7 +1995,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="19" thickBot="1">
+    <row r="56" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>113</v>
       </c>
@@ -1991,7 +2006,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="19" thickBot="1">
+    <row r="57" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>116</v>
       </c>
@@ -2000,7 +2015,7 @@
       </c>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:6" ht="19" thickBot="1">
+    <row r="58" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>118</v>
       </c>
@@ -2009,7 +2024,7 @@
       </c>
       <c r="C58" s="5"/>
     </row>
-    <row r="59" spans="1:6" ht="19" thickBot="1">
+    <row r="59" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>120</v>
       </c>
@@ -2029,21 +2044,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4343E511-C84F-5348-B9E4-371C584CD8FF}">
-  <dimension ref="A1:D52"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="167" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>132</v>
       </c>
@@ -2056,8 +2072,11 @@
       <c r="D1" s="13" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2070,21 +2089,36 @@
       <c r="D2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="C3" t="s">
-        <v>137</v>
-      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>160</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>158</v>
+      </c>
+      <c r="E4">
+        <v>245</v>
+      </c>
+      <c r="F4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2092,21 +2126,21 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" t="s">
         <v>140</v>
       </c>
-      <c r="D6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2114,61 +2148,79 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9">
+        <v>165</v>
+      </c>
+      <c r="F9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="14">
+      <c r="F10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="14">
         <v>2147483647</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="C11" t="s">
+      <c r="F11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12">
+        <v>-2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>143</v>
-      </c>
-      <c r="D11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="C12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12">
-        <v>-2147483647</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="C13" t="s">
-        <v>147</v>
       </c>
       <c r="D13">
         <v>-2147483647</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="F13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D14">
         <v>-2147483648</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="F14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>142</v>
+      </c>
+      <c r="F15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2176,61 +2228,79 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>163</v>
+      </c>
+      <c r="F17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D18" s="14">
+        <v>148</v>
+      </c>
+      <c r="D18" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="14">
         <v>2147483647</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="C19" t="s">
+      <c r="F19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20">
+        <v>-2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>143</v>
-      </c>
-      <c r="D19">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="C20" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20">
-        <v>-2147483647</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="C21" t="s">
-        <v>147</v>
       </c>
       <c r="D21">
         <v>-2147483647</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="F21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>142</v>
+      </c>
+      <c r="F22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>142</v>
+      </c>
+      <c r="F23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -2238,220 +2308,269 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
-      </c>
-      <c r="D25">
+        <v>163</v>
+      </c>
+      <c r="F25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="C26" t="s">
-        <v>151</v>
-      </c>
-      <c r="D26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="F26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>153</v>
-      </c>
-      <c r="D27">
+        <v>147</v>
+      </c>
+      <c r="D27" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28">
         <v>-32769</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="C28" t="s">
-        <v>154</v>
-      </c>
-      <c r="D28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
+      <c r="F28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>6</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>8</v>
       </c>
-      <c r="C30" t="s">
-        <v>152</v>
-      </c>
-      <c r="D30" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
       <c r="C31" t="s">
-        <v>150</v>
-      </c>
-      <c r="D31" s="14">
+        <v>148</v>
+      </c>
+      <c r="D31" t="s">
+        <v>142</v>
+      </c>
+      <c r="F31" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="14">
         <v>1879113727</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="C32" t="s">
-        <v>151</v>
-      </c>
-      <c r="D32">
+      <c r="F32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33">
         <v>-2147450882</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="C33" t="s">
-        <v>146</v>
-      </c>
-      <c r="D33">
-        <v>-2147483647</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="F33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D34">
         <v>-2147483647</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="F34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="C36" t="s">
-        <v>149</v>
-      </c>
-      <c r="D36" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38">
+        <v>142</v>
+      </c>
+      <c r="F35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>7</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B37" t="s">
         <v>103</v>
       </c>
+      <c r="C37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40">
+        <v>-2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" t="s">
+        <v>142</v>
+      </c>
+      <c r="F41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>155</v>
       </c>
-      <c r="D38">
+      <c r="D42" t="s">
+        <v>142</v>
+      </c>
+      <c r="F42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>157</v>
+      </c>
+      <c r="D43" t="s">
+        <v>142</v>
+      </c>
+      <c r="F43" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" t="s">
+        <v>151</v>
+      </c>
+      <c r="D45">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="C39" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>154</v>
+      </c>
+      <c r="D48">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>156</v>
       </c>
-      <c r="D39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="C40" t="s">
+      <c r="D49">
+        <v>2147483647</v>
+      </c>
+      <c r="F49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" t="s">
+        <v>142</v>
+      </c>
+      <c r="F50" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
         <v>157</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="C41" t="s">
-        <v>158</v>
-      </c>
-      <c r="D41">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="C42" t="s">
-        <v>160</v>
-      </c>
-      <c r="D42" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="C43" t="s">
-        <v>159</v>
-      </c>
-      <c r="D43" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="C44" t="s">
-        <v>161</v>
-      </c>
-      <c r="D44" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46">
-        <v>8</v>
-      </c>
-      <c r="B46" t="s">
-        <v>105</v>
-      </c>
-      <c r="C46" t="s">
-        <v>155</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="C47" t="s">
-        <v>156</v>
-      </c>
-      <c r="D47" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="C48" t="s">
-        <v>157</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="3:4">
-      <c r="C49" t="s">
-        <v>158</v>
-      </c>
-      <c r="D49">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4">
-      <c r="C50" t="s">
-        <v>160</v>
-      </c>
-      <c r="D50">
-        <v>2147483647</v>
-      </c>
-    </row>
-    <row r="51" spans="3:4">
-      <c r="C51" t="s">
-        <v>159</v>
-      </c>
-      <c r="D51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4">
-      <c r="C52" t="s">
-        <v>161</v>
-      </c>
-      <c r="D52">
+      <c r="D51">
         <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>